<commit_message>
deleted puzzles with irregular (multi char per cell) answers because we hate those
</commit_message>
<xml_diff>
--- a/data/puzzle_samples/blank_template.xlsx
+++ b/data/puzzle_samples/blank_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\witzi\OneDrive\Documents\neu_part_2\CS5100_FAI\code\ai_crossword_solver\data\puzzle_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F55C5C2-97D8-4EB8-87BC-30EFECFD4BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6CFE00-EFD6-4F06-9906-700D8D581757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2196" yWindow="5868" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>number</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>clue</t>
+  </si>
+  <si>
+    <t>length (optional column, for checking only)</t>
+  </si>
+  <si>
+    <t>answer (optional column, for checking only)</t>
   </si>
 </sst>
 </file>
@@ -360,15 +366,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,6 +392,12 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>